<commit_message>
beton update die zweite
</commit_message>
<xml_diff>
--- a/Baumaterial.xlsx
+++ b/Baumaterial.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="122">
   <si>
     <t>Keller</t>
   </si>
@@ -366,20 +366,51 @@
     <t>4:1 kies:zement  300-400kg zement/m³</t>
   </si>
   <si>
-    <t>4 m³ x 2 = ca.  2,4t</t>
-  </si>
-  <si>
     <t xml:space="preserve">ca 2t/m³ </t>
   </si>
   <si>
     <t>16t</t>
+  </si>
+  <si>
+    <t>ca.  2,4t = 96 Sack</t>
+  </si>
+  <si>
+    <t>4 m³ x 2 = 8 m³</t>
+  </si>
+  <si>
+    <t>Kosten</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">96 * </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3 = 288€</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,6 +430,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -735,23 +773,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -762,47 +801,50 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E9" s="4" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -812,19 +854,19 @@
       <c r="C11" t="s">
         <v>110</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -832,33 +874,39 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>121</v>
       </c>
       <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E15" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>114</v>
       </c>
     </row>
@@ -930,7 +978,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
@@ -938,23 +986,23 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>15</v>
       </c>
@@ -962,50 +1010,51 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>24</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>56</v>
       </c>
@@ -1178,37 +1227,38 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C86" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D86" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
-    <hyperlink ref="E9" r:id="rId2"/>
-    <hyperlink ref="E11" r:id="rId3"/>
-    <hyperlink ref="E12" r:id="rId4"/>
+    <hyperlink ref="F10" r:id="rId1"/>
+    <hyperlink ref="F9" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId5"/>

</xml_diff>